<commit_message>
Documentation for Sprint 2
</commit_message>
<xml_diff>
--- a/Documentation/Sprint_Review_Protocol_2.xlsx
+++ b/Documentation/Sprint_Review_Protocol_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sczer\Documents\3.Semester\INNO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kleme\OneDrive\Dokumente\1Technikum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10C206E3-F9A9-49D4-95EF-3C13F3B376F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0420C83-277F-4FD0-8ECF-0CACD6807C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Redl Chistoph</t>
+  </si>
+  <si>
+    <t>Shooting und Bewegung Verknüpfen</t>
   </si>
 </sst>
 </file>
@@ -378,6 +381,39 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -396,12 +432,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -415,38 +445,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -462,7 +465,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -761,10 +764,10 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="2" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" style="2" customWidth="1"/>
@@ -777,28 +780,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -812,131 +815,131 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="20">
+      <c r="B4" s="28"/>
+      <c r="C4" s="29">
         <v>1</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="33"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="23">
+      <c r="B6" s="16"/>
+      <c r="C6" s="32">
         <v>27</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="24"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="14" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="26"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="31" t="s">
+      <c r="B11" s="16"/>
+      <c r="C11" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="22"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="25" t="s">
+      <c r="B12" s="18"/>
+      <c r="C12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="27"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -966,14 +969,20 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <v>1</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="7">
+        <v>4</v>
+      </c>
+      <c r="D16" s="7">
+        <v>3</v>
+      </c>
       <c r="E16" s="9">
         <f>D16-C16</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="4"/>
@@ -1124,7 +1133,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6">
         <f>SUM(E16:E25)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F26" s="6">
         <f>COUNT(F16:F25)</f>
@@ -1149,12 +1158,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C11:G11"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -1169,6 +1172,12 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>